<commit_message>
Fine Tuned the System1 compoments from the Client Hash project
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/FrameworkTemplates/REFramework/VB/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A241907\Documents\UiPath\Generate_Yearly_Report\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FD469A-3FB0-4FBA-AA9C-1E542C9F01DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10248" yWindow="17508" windowWidth="21252" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -160,13 +160,25 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>EmailAccount</t>
+  </si>
+  <si>
+    <t>ACMECredentials</t>
+  </si>
+  <si>
+    <t>ACME_Credentials</t>
+  </si>
+  <si>
+    <t>kakoozaa2@stanbic.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -190,6 +202,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -208,10 +226,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -221,8 +240,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -538,15 +559,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -594,7 +615,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -604,7 +625,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -615,8 +636,22 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1610,8 +1645,11 @@
     <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{0541EFE9-124C-4BF2-876C-6CB84D3AF04F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1623,12 +1661,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1703,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1714,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1790,7 +1828,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2775,6 +2813,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2786,12 +2825,12 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3832,5 +3871,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Download Monthly Report Component
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A241907\Documents\UiPath\Generate_Yearly_Report\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FD469A-3FB0-4FBA-AA9C-1E542C9F01DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBDAB15-3544-4D8F-B0B7-1123361CC00B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -172,6 +172,18 @@
   </si>
   <si>
     <t>kakoozaa2@stanbic.com</t>
+  </si>
+  <si>
+    <t>DownloadsFolder</t>
+  </si>
+  <si>
+    <t>C:\Users\A241907\Downloads</t>
+  </si>
+  <si>
+    <t>C:\Users\A241907\Documents\UiPath\Generate_Yearly_Report\Data\Output</t>
+  </si>
+  <si>
+    <t>WorkFolder</t>
   </si>
 </sst>
 </file>
@@ -559,7 +571,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -652,8 +664,22 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Exception Handling and some fine tuning
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A241907\Documents\UiPath\Generate_Yearly_Report\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBDAB15-3544-4D8F-B0B7-1123361CC00B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C59FE04-8350-4C92-B0E9-176CF5D5770D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -177,13 +177,13 @@
     <t>DownloadsFolder</t>
   </si>
   <si>
-    <t>C:\Users\A241907\Downloads</t>
-  </si>
-  <si>
-    <t>C:\Users\A241907\Documents\UiPath\Generate_Yearly_Report\Data\Output</t>
-  </si>
-  <si>
     <t>WorkFolder</t>
+  </si>
+  <si>
+    <t>C:\Users\A241907\Downloads\</t>
+  </si>
+  <si>
+    <t>C:\Users\A241907\Documents\UiPath\Generate_Yearly_Report\Data\Output\</t>
   </si>
 </sst>
 </file>
@@ -571,7 +571,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -669,15 +669,15 @@
         <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
         <v>52</v>
-      </c>
-      <c r="B9" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>